<commit_message>
Add shops and healthbars
</commit_message>
<xml_diff>
--- a/MiniSvendeprøve/SvendDoc.xlsx
+++ b/MiniSvendeprøve/SvendDoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaspe\Desktop\H5Nr2\MiniSvendeprøve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6E32C3-0CBE-44FF-8412-5FB37CBA4D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43F6D81-C5E7-4BD9-8C6C-1C0884983F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{0EB5BA1A-1791-422F-AF2D-E00DBE5DD862}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11835" xr2:uid="{0EB5BA1A-1791-422F-AF2D-E00DBE5DD862}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Dag 1</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>Kom til at bytte om på 2 varaibler I spawn unit funktion på serveren. Debuggede I lang tid.</t>
+  </si>
+  <si>
+    <t>Fiksede civilization og arbejde på at lave en masse units</t>
+  </si>
+  <si>
+    <t>… Brugte meget lang tid på at få 1 label til at opdatere. Det var button prefabs som referenced til shop prefabs hvilket ikke er instantiated</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +276,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -461,6 +473,8 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,7 +802,7 @@
   <dimension ref="A2:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +906,8 @@
       <c r="H3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="34"/>
-      <c r="L3" s="10"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="37"/>
       <c r="N3" s="10"/>
       <c r="P3" s="2"/>
       <c r="R3" s="28"/>
@@ -914,7 +929,7 @@
       <c r="I4" s="20"/>
       <c r="J4" s="11"/>
       <c r="K4" s="35"/>
-      <c r="L4" s="11"/>
+      <c r="L4" s="30"/>
       <c r="M4" s="20"/>
       <c r="N4" s="11"/>
       <c r="O4" s="20"/>
@@ -976,50 +991,56 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
     </row>
   </sheetData>

</xml_diff>